<commit_message>
Eleven Store Ecommerce Project
</commit_message>
<xml_diff>
--- a/TestData/Mystoredata.xlsx
+++ b/TestData/Mystoredata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\MyStore\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98F67D8-F014-42FC-B8FF-E3A1ADF52520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F43CC8-3083-499B-92BE-3380789E5253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,25 +26,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>admin@123</t>
-  </si>
-  <si>
-    <t>admin@xyz.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postal</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>AlliensAddress</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Wankade</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Wankade,Mum</t>
+  </si>
+  <si>
+    <t>Shrithi</t>
+  </si>
+  <si>
+    <t>Mandana</t>
+  </si>
+  <si>
+    <t>kempa</t>
+  </si>
+  <si>
+    <t>banglore</t>
+  </si>
+  <si>
+    <t>kemp,bang</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Williamson</t>
+  </si>
+  <si>
+    <t>Kane</t>
+  </si>
+  <si>
+    <t>newzealand</t>
+  </si>
+  <si>
+    <t>willington</t>
+  </si>
+  <si>
+    <t>auckland</t>
+  </si>
+  <si>
+    <t>rohit@123</t>
+  </si>
+  <si>
+    <t>man@123</t>
+  </si>
+  <si>
+    <t>kane@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecommercetest@gmail.com	</t>
+  </si>
+  <si>
+    <t>etest@123</t>
+  </si>
+  <si>
+    <t>dreruss123@gmail.com</t>
+  </si>
+  <si>
+    <t>morgan789@gmail.com</t>
+  </si>
+  <si>
+    <t>dineshkarthik79@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,13 +169,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,14 +207,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,33 +501,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
     <col min="2" max="2" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{077D45BF-621C-462E-A07D-BADB776116FE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C6BD7273-FA29-490E-BC69-BC8720D6D790}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1A21D2-AD7A-45B4-8511-2A57B52CD3A9}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>2002</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>40056</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2">
+        <v>9877458740</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>2002</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>40055</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3">
+        <v>9877458740</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>2002</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>40055</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4">
+        <v>9877458740</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CE60453C-B6E4-44F7-BE24-7983F1F73957}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C269C2BB-0363-4E7A-AD00-66F6D553F5B7}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E09155C8-D543-47D7-B62F-5FDC3B8EC7FD}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{2AC5FB73-C512-443F-944E-79BF92AECC40}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{32A74B83-3B83-4E7F-8878-EDFBFAB7700D}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{6A8FA895-2DB3-41AD-B21E-18AEC5430230}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>